<commit_message>
Give users a sample Excel file to demonstrate correct formatting
Add sample Excel file generation with instructions for proper formatting.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ac2c2972-58d0-44f5-9684-cf1bc2f4174e
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/68b54b25-70f1-4bb2-b8d9-00d420c5379e/c10b3904-de0f-4a6f-80e0-1c611cd2fed7.jpg
</commit_message>
<xml_diff>
--- a/sample_images.xlsx
+++ b/sample_images.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sample Image Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sample Data" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,9 +28,29 @@
     </font>
     <font>
       <b val="1"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <i val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -38,8 +59,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="004472C4"/>
+        <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00E8F5E8"/>
         <bgColor rgb="00E8F5E8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F8F8F8"/>
+        <bgColor rgb="00F8F8F8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF2CC"/>
+        <bgColor rgb="00FFF2CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -55,9 +94,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -423,7 +467,282 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="59" customWidth="1" min="1" max="1"/>
+    <col width="2" customWidth="1" min="2" max="2"/>
+    <col width="2" customWidth="1" min="3" max="3"/>
+    <col width="2" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>SEO Alt Text Generator - Instructions</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr"/>
+      <c r="C1" s="1" t="inlineStr"/>
+      <c r="D1" s="1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>How to use this tool:</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>1. Your Excel file must have a column with image URLs</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>2. Column names that work for image URLs:</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - image_url</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - image</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - url</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - image_link</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>3. Optional: Alt text column (will be created if missing)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   Column names that work for alt text:</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - alt_text</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - alt</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - description</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - alt_description</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>4. You can include any other columns with additional data</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>5. The tool will:</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Automatically detect your image URL column</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Create an alt_text column if one doesn't exist</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Generate SEO-friendly alt text for missing entries</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Allow you to edit any generated text</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Export the updated file for download</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>See the 'Sample Data' sheet for an example format</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,39 +752,39 @@
   <cols>
     <col width="4" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="4" max="4"/>
     <col width="19" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="9" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Image URL</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Alt Text</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>image_url</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>alt_text</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
@@ -485,7 +804,7 @@
           <t>https://images.unsplash.com/photo-1494976688153-018c804d0dd7?w=800</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" s="5" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
           <t>Automotive</t>
@@ -511,7 +830,7 @@
           <t>https://images.unsplash.com/photo-1506905925346-21bda4d32df4?w=800</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="6" t="inlineStr">
         <is>
           <t>Beautiful mountain scenery with snow-capped peaks</t>
         </is>
@@ -541,7 +860,7 @@
           <t>https://images.unsplash.com/photo-1541167760496-1628856ab772?w=800</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" s="5" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>Food &amp; Drink</t>
@@ -567,7 +886,7 @@
           <t>https://images.unsplash.com/photo-1497366216548-37526070297c?w=800</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>Architecture</t>
@@ -593,7 +912,7 @@
           <t>https://images.unsplash.com/photo-1552053831-71594a27632d?w=800</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" s="5" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
           <t>Animals</t>
@@ -619,7 +938,7 @@
           <t>https://images.unsplash.com/photo-1540420773420-3366772f4999?w=800</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="6" t="inlineStr">
         <is>
           <t>Colorful fresh vegetables including tomatoes, peppers, and leafy greens</t>
         </is>
@@ -649,7 +968,7 @@
           <t>https://images.unsplash.com/photo-1449824913935-59a10b8d2000?w=800</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" s="5" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>Urban</t>
@@ -675,7 +994,7 @@
           <t>https://images.unsplash.com/photo-1506629905117-b5d1b8b6c4e5?w=800</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" s="5" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
           <t>Health &amp; Wellness</t>
@@ -684,58 +1003,6 @@
       <c r="F9" t="inlineStr">
         <is>
           <t>$25.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Beach Sunset</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>https://images.unsplash.com/photo-1507525428034-b723cf961d3e?w=800</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Nature</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Laptop Computer</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>https://images.unsplash.com/photo-1496181133206-80ce9b88a853?w=800</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Technology</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>$1,299.99</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Guide users to provide direct image URLs and improve URL validation
Adds direct image URL validation and updates sample data in Excel files.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: ac2c2972-58d0-44f5-9684-cf1bc2f4174e
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/68b54b25-70f1-4bb2-b8d9-00d420c5379e/7b63a450-bf71-49a9-81fd-acaaffdd150c.jpg
</commit_message>
<xml_diff>
--- a/sample_images.xlsx
+++ b/sample_images.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sample Data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sample Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,29 +27,17 @@
     </font>
     <font>
       <b val="1"/>
-      <sz val="16"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-      <sz val="16"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <i val="1"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
     <font>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00CC0000"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -61,24 +48,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="004472C4"/>
         <bgColor rgb="004472C4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E8F5E8"/>
-        <bgColor rgb="00E8F5E8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F8F8F8"/>
-        <bgColor rgb="00F8F8F8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFF2CC"/>
-        <bgColor rgb="00FFF2CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -94,14 +63,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -467,281 +432,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="59" customWidth="1" min="1" max="1"/>
-    <col width="2" customWidth="1" min="2" max="2"/>
-    <col width="2" customWidth="1" min="3" max="3"/>
-    <col width="2" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>SEO Alt Text Generator - Instructions</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr"/>
-      <c r="C1" s="1" t="inlineStr"/>
-      <c r="D1" s="1" t="inlineStr"/>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>How to use this tool:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>1. Your Excel file must have a column with image URLs</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>2. Column names that work for image URLs:</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - image_url</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - image</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - url</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - image_link</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>3. Optional: Alt text column (will be created if missing)</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   Column names that work for alt text:</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - alt_text</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - alt</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - description</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - alt_description</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>4. You can include any other columns with additional data</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>5. The tool will:</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Automatically detect your image URL column</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Create an alt_text column if one doesn't exist</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Generate SEO-friendly alt text for missing entries</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Allow you to edit any generated text</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Export the updated file for download</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>See the 'Sample Data' sheet for an example format</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -749,42 +439,34 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="4" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="60" customWidth="1" min="3" max="3"/>
-    <col width="60" customWidth="1" min="4" max="4"/>
-    <col width="19" customWidth="1" min="5" max="5"/>
-    <col width="9" customWidth="1" min="6" max="6"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>image_url</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>alt_text</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
@@ -796,23 +478,23 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Red Sports Car</t>
+          <t>Product Photo 1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://images.unsplash.com/photo-1494976688153-018c804d0dd7?w=800</t>
-        </is>
-      </c>
-      <c r="D2" s="5" t="inlineStr"/>
+          <t>https://example.com/image1.jpg</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Automotive</t>
+          <t>Products</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>$45,000</t>
+          <t>5.00</t>
         </is>
       </c>
     </row>
@@ -822,27 +504,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mountain Landscape</t>
+          <t>Lifestyle Image</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://images.unsplash.com/photo-1506905925346-21bda4d32df4?w=800</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>Beautiful mountain scenery with snow-capped peaks</t>
+          <t>https://example.com/image2.jpg</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>People enjoying outdoor activities</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Nature</t>
+          <t>Lifestyle</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>99.99</t>
         </is>
       </c>
     </row>
@@ -852,23 +534,23 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Coffee Cup</t>
+          <t>Brand Logo</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://images.unsplash.com/photo-1541167760496-1628856ab772?w=800</t>
-        </is>
-      </c>
-      <c r="D4" s="5" t="inlineStr"/>
+          <t>https://example.com/logo.png</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Food &amp; Drink</t>
+          <t>Branding</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$12.99</t>
+          <t>9.50</t>
         </is>
       </c>
     </row>
@@ -878,15 +560,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Modern Office</t>
+          <t>Building Photo</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://images.unsplash.com/photo-1497366216548-37526070297c?w=800</t>
-        </is>
-      </c>
-      <c r="D5" s="5" t="inlineStr"/>
+          <t>https://example.com/building.jpg</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>Architecture</t>
@@ -904,18 +586,18 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Golden Retriever</t>
+          <t>Nature Scene</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://images.unsplash.com/photo-1552053831-71594a27632d?w=800</t>
-        </is>
-      </c>
-      <c r="D6" s="5" t="inlineStr"/>
+          <t>https://example.com/nature.jpg</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Animals</t>
+          <t>Nature</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -930,79 +612,34 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Fresh Vegetables</t>
+          <t>Tech Product</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://images.unsplash.com/photo-1540420773420-3366772f4999?w=800</t>
-        </is>
-      </c>
-      <c r="D7" s="6" t="inlineStr">
-        <is>
-          <t>Colorful fresh vegetables including tomatoes, peppers, and leafy greens</t>
+          <t>https://example.com/tech.jpg</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Modern smartphone with sleek design</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>Technology</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$8.50</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>City Skyline</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>https://images.unsplash.com/photo-1449824913935-59a10b8d2000?w=800</t>
-        </is>
-      </c>
-      <c r="D8" s="5" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Urban</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>N/A</t>
+          <t>99.00</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Yoga Class</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>https://images.unsplash.com/photo-1506629905117-b5d1b8b6c4e5?w=800</t>
-        </is>
-      </c>
-      <c r="D9" s="5" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Health &amp; Wellness</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>$25.00</t>
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>NOTE: Replace example.com URLs with your actual image URLs</t>
         </is>
       </c>
     </row>

</xml_diff>